<commit_message>
Master log data testing
</commit_message>
<xml_diff>
--- a/sample_data/master_log.xlsx
+++ b/sample_data/master_log.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,6 +765,604 @@
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" t="n">
+        <v>220</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Tempo</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L5" t="n">
+        <v>150</v>
+      </c>
+      <c r="M5" t="n">
+        <v>300</v>
+      </c>
+      <c r="N5" t="n">
+        <v>80</v>
+      </c>
+      <c r="O5" t="n">
+        <v>50</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>8</v>
+      </c>
+      <c r="R5" t="n">
+        <v>70</v>
+      </c>
+      <c r="S5" t="n">
+        <v>50</v>
+      </c>
+      <c r="T5" t="n">
+        <v>8</v>
+      </c>
+      <c r="U5" t="n">
+        <v>9</v>
+      </c>
+      <c r="V5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" t="n">
+        <v>30</v>
+      </c>
+      <c r="X5" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>2400</v>
+      </c>
+      <c r="L6" t="n">
+        <v>140</v>
+      </c>
+      <c r="M6" t="n">
+        <v>280</v>
+      </c>
+      <c r="N6" t="n">
+        <v>75</v>
+      </c>
+      <c r="O6" t="n">
+        <v>45</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1900</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>69.8</v>
+      </c>
+      <c r="S6" t="n">
+        <v>52</v>
+      </c>
+      <c r="T6" t="n">
+        <v>7</v>
+      </c>
+      <c r="U6" t="n">
+        <v>8</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3</v>
+      </c>
+      <c r="W6" t="n">
+        <v>25</v>
+      </c>
+      <c r="X6" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>180</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Recovery</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>2300</v>
+      </c>
+      <c r="L7" t="n">
+        <v>130</v>
+      </c>
+      <c r="M7" t="n">
+        <v>260</v>
+      </c>
+      <c r="N7" t="n">
+        <v>70</v>
+      </c>
+      <c r="O7" t="n">
+        <v>40</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="R7" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>48</v>
+      </c>
+      <c r="T7" t="n">
+        <v>9</v>
+      </c>
+      <c r="U7" t="n">
+        <v>9</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" t="n">
+        <v>20</v>
+      </c>
+      <c r="X7" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45234</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>12</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Tempo</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>2600</v>
+      </c>
+      <c r="L8" t="n">
+        <v>160</v>
+      </c>
+      <c r="M8" t="n">
+        <v>320</v>
+      </c>
+      <c r="N8" t="n">
+        <v>85</v>
+      </c>
+      <c r="O8" t="n">
+        <v>55</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2100</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>7</v>
+      </c>
+      <c r="R8" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>55</v>
+      </c>
+      <c r="T8" t="n">
+        <v>6</v>
+      </c>
+      <c r="U8" t="n">
+        <v>7</v>
+      </c>
+      <c r="V8" t="n">
+        <v>4</v>
+      </c>
+      <c r="W8" t="n">
+        <v>35</v>
+      </c>
+      <c r="X8" t="n">
+        <v>70</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" t="n">
+        <v>240</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Interval</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>2700</v>
+      </c>
+      <c r="L9" t="n">
+        <v>170</v>
+      </c>
+      <c r="M9" t="n">
+        <v>340</v>
+      </c>
+      <c r="N9" t="n">
+        <v>90</v>
+      </c>
+      <c r="O9" t="n">
+        <v>60</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2200</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>8</v>
+      </c>
+      <c r="R9" t="n">
+        <v>69</v>
+      </c>
+      <c r="S9" t="n">
+        <v>53</v>
+      </c>
+      <c r="T9" t="n">
+        <v>8</v>
+      </c>
+      <c r="U9" t="n">
+        <v>8</v>
+      </c>
+      <c r="V9" t="n">
+        <v>2</v>
+      </c>
+      <c r="W9" t="n">
+        <v>40</v>
+      </c>
+      <c r="X9" t="n">
+        <v>80</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Long Run</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L10" t="n">
+        <v>150</v>
+      </c>
+      <c r="M10" t="n">
+        <v>300</v>
+      </c>
+      <c r="N10" t="n">
+        <v>80</v>
+      </c>
+      <c r="O10" t="n">
+        <v>50</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>9</v>
+      </c>
+      <c r="R10" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="S10" t="n">
+        <v>50</v>
+      </c>
+      <c r="T10" t="n">
+        <v>9</v>
+      </c>
+      <c r="U10" t="n">
+        <v>9</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W10" t="n">
+        <v>30</v>
+      </c>
+      <c r="X10" t="n">
+        <v>60</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Rest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>2200</v>
+      </c>
+      <c r="L11" t="n">
+        <v>120</v>
+      </c>
+      <c r="M11" t="n">
+        <v>240</v>
+      </c>
+      <c r="N11" t="n">
+        <v>65</v>
+      </c>
+      <c r="O11" t="n">
+        <v>35</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1700</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>10</v>
+      </c>
+      <c r="R11" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="S11" t="n">
+        <v>45</v>
+      </c>
+      <c r="T11" t="n">
+        <v>10</v>
+      </c>
+      <c r="U11" t="n">
+        <v>10</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>15</v>
+      </c>
+      <c r="X11" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>35</v>
+      </c>
+      <c r="E12" t="n">
+        <v>200</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Sweet Spot</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>2400</v>
+      </c>
+      <c r="L12" t="n">
+        <v>140</v>
+      </c>
+      <c r="M12" t="n">
+        <v>280</v>
+      </c>
+      <c r="N12" t="n">
+        <v>75</v>
+      </c>
+      <c r="O12" t="n">
+        <v>45</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1900</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="R12" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="S12" t="n">
+        <v>51</v>
+      </c>
+      <c r="T12" t="n">
+        <v>7</v>
+      </c>
+      <c r="U12" t="n">
+        <v>8</v>
+      </c>
+      <c r="V12" t="n">
+        <v>3</v>
+      </c>
+      <c r="W12" t="n">
+        <v>25</v>
+      </c>
+      <c r="X12" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>250</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added phase ability to training log
</commit_message>
<xml_diff>
--- a/sample_data/master_log.xlsx
+++ b/sample_data/master_log.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM11"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,693 +641,136 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44927</v>
+        <v>45976</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Home</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>45975.29166666666</v>
+          <t>Indoor</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>07:00:00</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" t="n">
         <v>160</v>
       </c>
       <c r="I2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
         <v>5</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Good session</t>
+          <t>Felt good today</t>
         </is>
       </c>
       <c r="N2" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="O2" t="n">
+        <v>54</v>
+      </c>
+      <c r="P2" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>45</v>
+      </c>
+      <c r="R2" t="n">
+        <v>256</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>9</v>
+      </c>
+      <c r="V2" t="n">
+        <v>89</v>
+      </c>
+      <c r="W2" t="n">
+        <v>76</v>
+      </c>
+      <c r="X2" t="n">
         <v>2</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>200</v>
-      </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
+      <c r="Y2" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AB2" t="n">
-        <v>250</v>
+        <v>376</v>
       </c>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
-        <v>2500</v>
-      </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>44928</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Build</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Trail</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45975.27083333334</v>
-      </c>
-      <c r="F3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>48</v>
-      </c>
-      <c r="H3" t="n">
-        <v>160</v>
-      </c>
-      <c r="I3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" t="n">
-        <v>7</v>
-      </c>
-      <c r="K3" t="n">
-        <v>6</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Tired</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>3</v>
-      </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>220</v>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>250</v>
-      </c>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>2600</v>
-      </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Peak</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Gym</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45975.30208333334</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" t="n">
-        <v>52</v>
-      </c>
-      <c r="H4" t="n">
-        <v>160</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K4" t="n">
-        <v>8</v>
-      </c>
-      <c r="L4" t="n">
-        <v>6</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Strong</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>180</v>
-      </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>250</v>
-      </c>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="n">
-        <v>2400</v>
-      </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>44930</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Taper</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Road</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>45975.28125</v>
-      </c>
-      <c r="F5" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>49</v>
-      </c>
-      <c r="H5" t="n">
-        <v>160</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J5" t="n">
-        <v>6</v>
-      </c>
-      <c r="K5" t="n">
-        <v>5</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Recovery</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
-        <v>250</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>250</v>
-      </c>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="n">
-        <v>2700</v>
-      </c>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>44931</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Race</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Track</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>45975.3125</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" t="n">
-        <v>51</v>
-      </c>
-      <c r="H6" t="n">
-        <v>160</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8</v>
-      </c>
-      <c r="J6" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" t="n">
-        <v>7</v>
-      </c>
-      <c r="L6" t="n">
-        <v>5</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>PR</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>210</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>250</v>
-      </c>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="n">
-        <v>2550</v>
-      </c>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>0.3913888888888889</v>
-      </c>
-      <c r="O7" t="n">
-        <v>5.796069091601068</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="n">
-        <v>92.80000000000072</v>
-      </c>
-      <c r="R7" t="n">
-        <v>140.1695035460993</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>0.3913888888888889</v>
-      </c>
-      <c r="O8" t="n">
-        <v>5.796069091601068</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="n">
-        <v>92.80000000000072</v>
-      </c>
-      <c r="R8" t="n">
-        <v>140.1695035460993</v>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
-        <v>0.3913888888888889</v>
-      </c>
-      <c r="O9" t="n">
-        <v>5.796069091601068</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="n">
-        <v>92.80000000000072</v>
-      </c>
-      <c r="R9" t="n">
-        <v>140.1695035460993</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
-        <v>0.3913888888888889</v>
-      </c>
-      <c r="O10" t="n">
-        <v>5.796069091601068</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="n">
-        <v>92.80000000000072</v>
-      </c>
-      <c r="R10" t="n">
-        <v>140.1695035460993</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45974</v>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
-        <v>0.3913888888888889</v>
-      </c>
-      <c r="O11" t="n">
-        <v>5.796069091601068</v>
-      </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="n">
-        <v>92.80000000000072</v>
-      </c>
-      <c r="R11" t="n">
-        <v>140.1695035460993</v>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="inlineStr"/>
-      <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="inlineStr"/>
+        <v>4531</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>198</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>754</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>112</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>123</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>90</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added a log and testing debugger
</commit_message>
<xml_diff>
--- a/sample_data/master_log.xlsx
+++ b/sample_data/master_log.xlsx
@@ -19,10 +19,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -61,12 +58,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,45 +562,6 @@
           <t>Z5 Time (min)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cycling</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -617,7 +574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,28 +633,6 @@
           <t>Sodium intra (g)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>44928</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Running</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -710,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,36 +699,6 @@
           <t>Weight (lbs)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>44928</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -806,7 +711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -866,38 +771,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>44928</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
`Reordered and reordered columns in processed_master.csv and updated master_log.xlsx`
</commit_message>
<xml_diff>
--- a/sample_data/master_log.xlsx
+++ b/sample_data/master_log.xlsx
@@ -19,7 +19,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +565,93 @@
         <is>
           <t>Z5 Time (min)</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Build</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cycling</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Outdoors</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>56</v>
+      </c>
+      <c r="G2" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2" t="n">
+        <v>54</v>
+      </c>
+      <c r="I2" t="n">
+        <v>234</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Zone 2</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Mix</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>9</v>
+      </c>
+      <c r="M2" t="n">
+        <v>87</v>
+      </c>
+      <c r="N2" t="n">
+        <v>89</v>
+      </c>
+      <c r="O2" t="n">
+        <v>370</v>
+      </c>
+      <c r="P2" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S2" t="n">
+        <v>156</v>
+      </c>
+      <c r="T2" t="n">
+        <v>124</v>
+      </c>
+      <c r="U2" t="n">
+        <v>10</v>
+      </c>
+      <c r="V2" t="n">
+        <v>50</v>
+      </c>
+      <c r="W2" t="n">
+        <v>60</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +722,41 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Sodium intra (g)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Max HR</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Avg HR</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Z1 Time (min)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Z2 Time (min)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Z3 Time (min)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Z4 Time (min)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Z5 Time (min)</t>
         </is>
       </c>
     </row>
@@ -645,7 +771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -699,6 +825,19 @@
           <t>Weight (lbs)</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -711,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,6 +910,20 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>